<commit_message>
New bumpers code that works
</commit_message>
<xml_diff>
--- a/Codes/Mega_bumpers/Pin_mapping.xlsx
+++ b/Codes/Mega_bumpers/Pin_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="13940" yWindow="0" windowWidth="11420" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mega" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,14 +501,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="23">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -824,16 +856,16 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C52" sqref="C52:C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>